<commit_message>
Gerrit K. zijn taken bijgewerkt
</commit_message>
<xml_diff>
--- a/doc/Andalusier documenten/Individuele taakverdeling/Gerrit K/Gerrit K. taken.xlsx
+++ b/doc/Andalusier documenten/Individuele taakverdeling/Gerrit K/Gerrit K. taken.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karin\Desktop\Andalusier documenten\Individuele taakverdeling\Gerrit K\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\xampp\htdocs\andalusier\doc\Andalusier documenten\Individuele taakverdeling\Gerrit K\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -189,7 +189,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +218,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0066"/>
         <bgColor rgb="FFE91D63"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0066"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -313,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -350,6 +356,8 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,7 +762,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -813,7 +821,7 @@
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="24"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
@@ -950,7 +958,7 @@
       <c r="E15" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="17"/>
+      <c r="F15" s="25"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">

</xml_diff>